<commit_message>
fields - add line
</commit_message>
<xml_diff>
--- a/configuration/fields.xlsx
+++ b/configuration/fields.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dedi\Desktop\עבודה\My GIS\דשא\מרץ 2024\עבודה\configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dedi\Desktop\עבודה\My GIS\דשא\מרץ 2024\עבודה\gitgit - test\configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A5E284-7416-4D64-9500-7C201D23F35A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FACC186-DE0C-4067-9183-93FA2081DFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="673" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="673" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fields" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'_fields old'!$A$1:$J$275</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">fields!$A$1:$G$294</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">fields!$A$1:$G$295</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2643" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2644" uniqueCount="429">
   <si>
     <t>OBJECTID</t>
   </si>
@@ -1346,6 +1346,9 @@
   <si>
     <t>סטטוס</t>
   </si>
+  <si>
+    <t>A brand new line right here</t>
+  </si>
 </sst>
 </file>
 
@@ -2473,8 +2476,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E43E37A3-7B67-4000-A29A-CE671685306A}" name="fields" displayName="fields" ref="A1:G294" totalsRowShown="0" dataDxfId="63">
-  <autoFilter ref="A1:G294" xr:uid="{E43E37A3-7B67-4000-A29A-CE671685306A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E43E37A3-7B67-4000-A29A-CE671685306A}" name="fields" displayName="fields" ref="A1:G295" totalsRowShown="0" dataDxfId="63">
+  <autoFilter ref="A1:G295" xr:uid="{E43E37A3-7B67-4000-A29A-CE671685306A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{55F41C63-F033-407F-8E01-E15B9BD574B1}" name="code" dataDxfId="62"/>
     <tableColumn id="5" xr3:uid="{1B1F22C4-6894-4A74-B995-BF7E12179554}" name="tableName(notinuse)" dataDxfId="61"/>
@@ -2944,9 +2947,9 @@
   </sheetPr>
   <dimension ref="A1:G305"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A270" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A288" sqref="A288:A294"/>
+      <selection pane="bottomLeft" activeCell="G298" sqref="G298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8742,9 +8745,10 @@
       </c>
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A295"/>
-      <c r="B295"/>
-      <c r="C295"/>
+      <c r="A295" s="43"/>
+      <c r="B295" s="16" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="296" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A296"/>
@@ -27335,8 +27339,8 @@
   </sheetPr>
   <dimension ref="A1:J294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B290" sqref="B290:H290"/>
+    <sheetView topLeftCell="A259" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B295" sqref="B295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
trying onedrive this evening
</commit_message>
<xml_diff>
--- a/configuration/fields.xlsx
+++ b/configuration/fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dedi\Desktop\עבודה\My GIS\דשא\מרץ 2024\עבודה\gitgit - test\configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FACC186-DE0C-4067-9183-93FA2081DFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0B4812-726D-4905-9ECB-C09F76BA0822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="673" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'_fields old'!$A$1:$J$275</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">fields!$A$1:$G$295</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">fields!$A$1:$G$294</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2644" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2643" uniqueCount="428">
   <si>
     <t>OBJECTID</t>
   </si>
@@ -1346,9 +1346,6 @@
   <si>
     <t>סטטוס</t>
   </si>
-  <si>
-    <t>A brand new line right here</t>
-  </si>
 </sst>
 </file>
 
@@ -2476,8 +2473,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E43E37A3-7B67-4000-A29A-CE671685306A}" name="fields" displayName="fields" ref="A1:G295" totalsRowShown="0" dataDxfId="63">
-  <autoFilter ref="A1:G295" xr:uid="{E43E37A3-7B67-4000-A29A-CE671685306A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E43E37A3-7B67-4000-A29A-CE671685306A}" name="fields" displayName="fields" ref="A1:G294" totalsRowShown="0" dataDxfId="63">
+  <autoFilter ref="A1:G294" xr:uid="{E43E37A3-7B67-4000-A29A-CE671685306A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{55F41C63-F033-407F-8E01-E15B9BD574B1}" name="code" dataDxfId="62"/>
     <tableColumn id="5" xr3:uid="{1B1F22C4-6894-4A74-B995-BF7E12179554}" name="tableName(notinuse)" dataDxfId="61"/>
@@ -2945,11 +2942,11 @@
     <tabColor theme="0" tint="-0.499984740745262"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G305"/>
+  <dimension ref="A1:G304"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A270" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G298" sqref="G298"/>
+      <selection pane="bottomLeft" activeCell="E296" sqref="E296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8745,10 +8742,9 @@
       </c>
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A295" s="43"/>
-      <c r="B295" s="16" t="s">
-        <v>428</v>
-      </c>
+      <c r="A295"/>
+      <c r="B295"/>
+      <c r="C295"/>
     </row>
     <row r="296" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A296"/>
@@ -8794,11 +8790,6 @@
       <c r="A304"/>
       <c r="B304"/>
       <c r="C304"/>
-    </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A305"/>
-      <c r="B305"/>
-      <c r="C305"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>

</xml_diff>